<commit_message>
Sistema de submissao já gerando o cronograma de 2016.2.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Monitores.xlsx
+++ b/leda-submission-server/conf/Monitores.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Matricula</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>Monitor 1</t>
+  </si>
+  <si>
+    <t>Monitor 2</t>
+  </si>
+  <si>
+    <t>monitor1@gmail.com</t>
+  </si>
+  <si>
+    <t>monitor2@gmail.com</t>
+  </si>
+  <si>
+    <t>4567</t>
   </si>
 </sst>
 </file>
@@ -355,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -390,6 +402,20 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Retirada de pequenos erros na construcao do cronograma.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Monitores.xlsx
+++ b/leda-submission-server/conf/Monitores.xlsx
@@ -18,8 +18,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>cursou EDA e LEDA ha muito tempo.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Matricula</t>
   </si>
@@ -33,26 +55,128 @@
     <t>Fone</t>
   </si>
   <si>
-    <t>Monitor 1</t>
-  </si>
-  <si>
-    <t>Monitor 2</t>
-  </si>
-  <si>
-    <t>monitor1@gmail.com</t>
-  </si>
-  <si>
-    <t>monitor2@gmail.com</t>
-  </si>
-  <si>
-    <t>4567</t>
+    <t>Tipo de Participacao</t>
+  </si>
+  <si>
+    <t>Tipo de Monitor</t>
+  </si>
+  <si>
+    <t>Horario de preferência (se não tiver preferência, deixe em branco)</t>
+  </si>
+  <si>
+    <t>Disponibilidade</t>
+  </si>
+  <si>
+    <t>Marcos Williams Cavalcanti de Arruda</t>
+  </si>
+  <si>
+    <t>marcos.arruda@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>DID 1</t>
+  </si>
+  <si>
+    <t>Corretor</t>
+  </si>
+  <si>
+    <t>Gabriel Morais Lucio de Araujo</t>
+  </si>
+  <si>
+    <t>gabmla19@gmail.com</t>
+  </si>
+  <si>
+    <t>DID 2</t>
+  </si>
+  <si>
+    <t>Vélmer Oliveira Odon</t>
+  </si>
+  <si>
+    <t>velmer.odon@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>83 98633-6857</t>
+  </si>
+  <si>
+    <t>Francisco Angelim de Figueirêdo Filho</t>
+  </si>
+  <si>
+    <t>francisco.filho@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>(83) 8621-5252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ytalo luiz Ouriques Rodrigues </t>
+  </si>
+  <si>
+    <t>ytalo.rodrigues@ccc.ufcg.edu</t>
+  </si>
+  <si>
+    <t>Anarco Quaresma Zeferino Nascimento</t>
+  </si>
+  <si>
+    <t>anarco.nascimento@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>83 9 96796979</t>
+  </si>
+  <si>
+    <t>Desenvolvedor</t>
+  </si>
+  <si>
+    <t>Laybson Plismenn Sousa Cunha</t>
+  </si>
+  <si>
+    <t>laybson.cunha@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>Antunes Dantas da Silva</t>
+  </si>
+  <si>
+    <t>antunes.silva@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>Lucas Henrique de Lima e Silva</t>
+  </si>
+  <si>
+    <t>lucas.silva@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>81 998054501</t>
+  </si>
+  <si>
+    <t>Igor de Araújo Meira</t>
+  </si>
+  <si>
+    <t>igor.meira@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(83)987272773 </t>
+  </si>
+  <si>
+    <t>Daniyel Negromonte Nascimento Rocha</t>
+  </si>
+  <si>
+    <t>daniyel.rocha@ccc.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>(73) 98828-4680</t>
+  </si>
+  <si>
+    <t>Bolsa</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>Lucas Cavalcanti Rodrigues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -62,16 +186,31 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -79,14 +218,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,6 +282,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,22 +594,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -394,31 +623,262 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1234</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>114210695</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6">
+        <v>83999900395</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>114111359</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8333320610</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>115110575</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>115111033</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>114210821</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6">
+        <v>83999302796</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>114110419</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>114210198</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="6">
+        <v>998309861</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>115110295</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="6">
+        <v>83998695646</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>115110163</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>112210079</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>114210779</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>114211200</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao para suportar senhas.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/Monitores.xlsx
+++ b/leda-submission-server/conf/Monitores.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
   <si>
     <t>Matricula</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>(83) 998272800</t>
+  </si>
+  <si>
+    <t>Senha</t>
   </si>
 </sst>
 </file>
@@ -312,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -363,11 +366,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -411,6 +425,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,6 +477,54 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
@@ -739,25 +806,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1002"/>
+  <dimension ref="A1:I1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
     <col min="8" max="8" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,8 +849,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>115111901</v>
       </c>
@@ -808,8 +878,11 @@
       <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="4">
+        <v>115111901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>114110419</v>
       </c>
@@ -834,8 +907,11 @@
       <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="4">
+        <v>114110419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>115111271</v>
       </c>
@@ -860,8 +936,11 @@
       <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="4">
+        <v>115111271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>115110295</v>
       </c>
@@ -886,8 +965,11 @@
       <c r="H5" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="4">
+        <v>115110295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>114210779</v>
       </c>
@@ -912,8 +994,11 @@
       <c r="H6" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="4">
+        <v>114210779</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>115111033</v>
       </c>
@@ -936,8 +1021,11 @@
       <c r="H7" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="4">
+        <v>115111033</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>114111359</v>
       </c>
@@ -960,8 +1048,11 @@
       <c r="H8" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="4">
+        <v>114111359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>112210079</v>
       </c>
@@ -986,8 +1077,11 @@
       <c r="H9" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="4">
+        <v>112210079</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>114210198</v>
       </c>
@@ -1010,8 +1104,11 @@
       <c r="H10" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="4">
+        <v>114210198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>114211200</v>
       </c>
@@ -1036,8 +1133,11 @@
       <c r="H11" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="4">
+        <v>114211200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>115110163</v>
       </c>
@@ -1062,8 +1162,11 @@
       <c r="H12" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="4">
+        <v>115110163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>115110721</v>
       </c>
@@ -1088,8 +1191,11 @@
       <c r="H13" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="4">
+        <v>115110721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>114210695</v>
       </c>
@@ -1112,8 +1218,11 @@
       <c r="H14" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="4">
+        <v>114210695</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>113110905</v>
       </c>
@@ -1138,8 +1247,11 @@
       <c r="H15" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="4">
+        <v>113110905</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>115110575</v>
       </c>
@@ -1152,18 +1264,21 @@
       <c r="D16" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5" t="s">
+      <c r="G16" s="14"/>
+      <c r="H16" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="13">
+        <v>115110575</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <v>1610274</v>
       </c>
@@ -1176,9 +1291,15 @@
       <c r="D17" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="16">
+        <v>1610274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16">
         <v>2051962</v>
       </c>
@@ -1191,74 +1312,80 @@
       <c r="D18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="16">
+        <v>2051962</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>

</xml_diff>